<commit_message>
chore: price table and contact in landing, delete in contexts orders, reports
</commit_message>
<xml_diff>
--- a/public/docs/import-student-orders.xlsx
+++ b/public/docs/import-student-orders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACN\tsa-frontend\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FB0213-E395-44DC-A91A-91B9CB7113CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5217E2-E62F-4D6F-8A2E-24CFF025E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,13 +99,13 @@
     <t>Lazada</t>
   </si>
   <si>
-    <t>MU1</t>
-  </si>
-  <si>
-    <t>MU2</t>
-  </si>
-  <si>
-    <t>MU3</t>
+    <t>TU1</t>
+  </si>
+  <si>
+    <t>TU2</t>
+  </si>
+  <si>
+    <t>TU3</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>